<commit_message>
I may have got in to bad habits vis-a-vis commits
</commit_message>
<xml_diff>
--- a/data/raw/Statistics_Norway/WWTP_by_County_2020_Small.xlsx
+++ b/data/raw/Statistics_Norway/WWTP_by_County_2020_Small.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/346ebfb30976329f/Projects/Papers/99_Thesis/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/346ebfb30976329f/Projects/Papers/03_Bayesian_Mixture_Toxicity/API_RQ_BN/data/raw/Statistics_Norway/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_F71CBCE1D837C17A77E613D9878B33B3EC921268" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_F71CBCE1D837C17A77E613D9878B33B3EC921268" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5450007B-278D-4E24-B601-763A1FB47B84}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-6792" windowWidth="17496" windowHeight="30336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Personer" sheetId="2" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>34 Innlandet</t>
   </si>
   <si>
-    <t>38 Vestfold og Telemark</t>
-  </si>
-  <si>
     <t>42 Agder</t>
   </si>
   <si>
@@ -152,18 +149,12 @@
     <t>46 Vestland</t>
   </si>
   <si>
-    <t>15 Møre og Romsdal</t>
-  </si>
-  <si>
     <t>50 Trøndelag - Trööndelage</t>
   </si>
   <si>
     <t>18 Nordland - Nordlánnda</t>
   </si>
   <si>
-    <t>54 Troms og Finnmark - Romsa ja Finnmárku</t>
-  </si>
-  <si>
     <t>.. = Data not available. Figures have not been entered into our databases or are too unreliable to be published.</t>
   </si>
   <si>
@@ -249,6 +240,15 @@
   </si>
   <si>
     <t>Personer</t>
+  </si>
+  <si>
+    <t>38 Vestfold &amp; Telemark</t>
+  </si>
+  <si>
+    <t>15 Møre &amp; Romsdal</t>
+  </si>
+  <si>
+    <t>54 Troms &amp; Finnmark - Romsa ja Finnmárku</t>
   </si>
 </sst>
 </file>
@@ -305,16 +305,16 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,932 +619,935 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="139.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>116241</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>324</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>35460</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>988</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>1247</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>30228</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>28888</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>4327</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <v>4059</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <v>2363</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="3">
         <v>2193</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="3">
         <v>281</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="3">
         <v>4601</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="3">
         <v>487</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="3">
         <v>795</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>1922</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>361</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>205</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="3">
         <v>18</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="3">
         <v>32</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="3">
         <v>2</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="3">
         <v>1025</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="3">
         <v>59</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="3">
         <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>115405</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>625</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>9220</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>79</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>152</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>2249</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>83565</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>2347</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="3">
         <v>3027</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="3">
         <v>111</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="3">
         <v>1101</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="3">
         <v>2</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="3">
         <v>10304</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="3">
         <v>84</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="3">
         <v>2539</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="3">
+        <v>56006</v>
+      </c>
+      <c r="C9" s="3">
+        <v>486</v>
+      </c>
+      <c r="D9" s="3">
+        <v>23448</v>
+      </c>
+      <c r="E9" s="3">
+        <v>651</v>
+      </c>
+      <c r="F9" s="3">
+        <v>241</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4126</v>
+      </c>
+      <c r="H9" s="3">
+        <v>16842</v>
+      </c>
+      <c r="I9" s="3">
+        <v>5787</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1373</v>
+      </c>
+      <c r="K9" s="3">
+        <v>30</v>
+      </c>
+      <c r="L9" s="3">
+        <v>765</v>
+      </c>
+      <c r="M9" s="3">
+        <v>70</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1712</v>
+      </c>
+      <c r="O9" s="3">
+        <v>3</v>
+      </c>
+      <c r="P9" s="3">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5">
-        <v>56006</v>
-      </c>
-      <c r="C9" s="5">
-        <v>486</v>
-      </c>
-      <c r="D9" s="5">
-        <v>23448</v>
-      </c>
-      <c r="E9" s="5">
-        <v>651</v>
-      </c>
-      <c r="F9" s="5">
-        <v>241</v>
-      </c>
-      <c r="G9" s="5">
-        <v>4126</v>
-      </c>
-      <c r="H9" s="5">
-        <v>16842</v>
-      </c>
-      <c r="I9" s="5">
-        <v>5787</v>
-      </c>
-      <c r="J9" s="5">
-        <v>1373</v>
-      </c>
-      <c r="K9" s="5">
+      <c r="B10" s="3">
+        <v>44078</v>
+      </c>
+      <c r="C10" s="3">
+        <v>966</v>
+      </c>
+      <c r="D10" s="3">
+        <v>12808</v>
+      </c>
+      <c r="E10" s="3">
+        <v>657</v>
+      </c>
+      <c r="F10" s="3">
+        <v>260</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3500</v>
+      </c>
+      <c r="H10" s="3">
+        <v>21214</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1810</v>
+      </c>
+      <c r="J10" s="3">
+        <v>672</v>
+      </c>
+      <c r="K10" s="3">
+        <v>355</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1189</v>
+      </c>
+      <c r="M10" s="3">
+        <v>48</v>
+      </c>
+      <c r="N10" s="3">
+        <v>476</v>
+      </c>
+      <c r="O10" s="3">
+        <v>93</v>
+      </c>
+      <c r="P10" s="3">
         <v>30</v>
       </c>
-      <c r="L9" s="5">
-        <v>765</v>
-      </c>
-      <c r="M9" s="5">
-        <v>70</v>
-      </c>
-      <c r="N9" s="5">
-        <v>1712</v>
-      </c>
-      <c r="O9" s="5">
-        <v>3</v>
-      </c>
-      <c r="P9" s="5">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="5">
-        <v>44078</v>
-      </c>
-      <c r="C10" s="5">
-        <v>966</v>
-      </c>
-      <c r="D10" s="5">
-        <v>12808</v>
-      </c>
-      <c r="E10" s="5">
-        <v>657</v>
-      </c>
-      <c r="F10" s="5">
-        <v>260</v>
-      </c>
-      <c r="G10" s="5">
-        <v>3500</v>
-      </c>
-      <c r="H10" s="5">
-        <v>21214</v>
-      </c>
-      <c r="I10" s="5">
-        <v>1810</v>
-      </c>
-      <c r="J10" s="5">
-        <v>672</v>
-      </c>
-      <c r="K10" s="5">
-        <v>355</v>
-      </c>
-      <c r="L10" s="5">
-        <v>1189</v>
-      </c>
-      <c r="M10" s="5">
-        <v>48</v>
-      </c>
-      <c r="N10" s="5">
-        <v>476</v>
-      </c>
-      <c r="O10" s="5">
-        <v>93</v>
-      </c>
-      <c r="P10" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="3">
+        <v>39826</v>
+      </c>
+      <c r="C11" s="3">
+        <v>710</v>
+      </c>
+      <c r="D11" s="3">
+        <v>28792</v>
+      </c>
+      <c r="E11" s="3">
+        <v>396</v>
+      </c>
+      <c r="F11" s="3">
+        <v>322</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1573</v>
+      </c>
+      <c r="H11" s="3">
+        <v>5820</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1446</v>
+      </c>
+      <c r="J11" s="3">
+        <v>84</v>
+      </c>
+      <c r="K11" s="3">
+        <v>58</v>
+      </c>
+      <c r="L11" s="3">
+        <v>269</v>
+      </c>
+      <c r="M11" s="3">
+        <v>192</v>
+      </c>
+      <c r="N11" s="3">
+        <v>59</v>
+      </c>
+      <c r="O11" s="3">
+        <v>23</v>
+      </c>
+      <c r="P11" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5">
-        <v>39826</v>
-      </c>
-      <c r="C11" s="5">
-        <v>710</v>
-      </c>
-      <c r="D11" s="5">
-        <v>28792</v>
-      </c>
-      <c r="E11" s="5">
-        <v>396</v>
-      </c>
-      <c r="F11" s="5">
-        <v>322</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1573</v>
-      </c>
-      <c r="H11" s="5">
-        <v>5820</v>
-      </c>
-      <c r="I11" s="5">
-        <v>1446</v>
-      </c>
-      <c r="J11" s="5">
+      <c r="B12" s="3">
+        <v>136615</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4175</v>
+      </c>
+      <c r="D12" s="3">
+        <v>77984</v>
+      </c>
+      <c r="E12" s="3">
+        <v>838</v>
+      </c>
+      <c r="F12" s="3">
+        <v>125</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5075</v>
+      </c>
+      <c r="H12" s="3">
+        <v>30956</v>
+      </c>
+      <c r="I12" s="3">
+        <v>16106</v>
+      </c>
+      <c r="J12" s="3">
+        <v>883</v>
+      </c>
+      <c r="K12" s="3">
+        <v>149</v>
+      </c>
+      <c r="L12" s="3">
+        <v>282</v>
+      </c>
+      <c r="M12" s="3">
+        <v>17</v>
+      </c>
+      <c r="N12" s="3">
+        <v>2</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="3">
+        <v>56287</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2031</v>
+      </c>
+      <c r="D13" s="3">
+        <v>38161</v>
+      </c>
+      <c r="E13" s="3">
+        <v>205</v>
+      </c>
+      <c r="F13" s="3">
+        <v>106</v>
+      </c>
+      <c r="G13" s="3">
+        <v>259</v>
+      </c>
+      <c r="H13" s="3">
+        <v>9667</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1739</v>
+      </c>
+      <c r="J13" s="3">
+        <v>146</v>
+      </c>
+      <c r="K13" s="3">
+        <v>39</v>
+      </c>
+      <c r="L13" s="3">
+        <v>743</v>
+      </c>
+      <c r="M13" s="3">
+        <v>690</v>
+      </c>
+      <c r="N13" s="3">
+        <v>328</v>
+      </c>
+      <c r="O13" s="3">
+        <v>82</v>
+      </c>
+      <c r="P13" s="3">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3">
+        <v>83191</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1135</v>
+      </c>
+      <c r="D14" s="3">
+        <v>35156</v>
+      </c>
+      <c r="E14" s="3">
+        <v>723</v>
+      </c>
+      <c r="F14" s="3">
+        <v>222</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1617</v>
+      </c>
+      <c r="H14" s="3">
+        <v>21082</v>
+      </c>
+      <c r="I14" s="3">
+        <v>16736</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1063</v>
+      </c>
+      <c r="K14" s="3">
+        <v>192</v>
+      </c>
+      <c r="L14" s="3">
+        <v>489</v>
+      </c>
+      <c r="M14" s="3">
+        <v>61</v>
+      </c>
+      <c r="N14" s="3">
+        <v>96</v>
+      </c>
+      <c r="O14" s="3">
+        <v>24</v>
+      </c>
+      <c r="P14" s="3">
+        <v>4595</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="3">
+        <v>72218</v>
+      </c>
+      <c r="C15" s="3">
+        <v>6617</v>
+      </c>
+      <c r="D15" s="3">
+        <v>45178</v>
+      </c>
+      <c r="E15" s="3">
+        <v>613</v>
+      </c>
+      <c r="F15" s="3">
+        <v>120</v>
+      </c>
+      <c r="G15" s="3">
+        <v>162</v>
+      </c>
+      <c r="H15" s="3">
+        <v>14982</v>
+      </c>
+      <c r="I15" s="3">
+        <v>4041</v>
+      </c>
+      <c r="J15" s="3">
+        <v>143</v>
+      </c>
+      <c r="K15" s="3">
+        <v>2</v>
+      </c>
+      <c r="L15" s="3">
+        <v>129</v>
+      </c>
+      <c r="M15" s="3">
+        <v>89</v>
+      </c>
+      <c r="N15" s="3">
+        <v>7</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P15" s="3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="3">
+        <v>54533</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5598</v>
+      </c>
+      <c r="D16" s="3">
+        <v>26944</v>
+      </c>
+      <c r="E16" s="3">
+        <v>71</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="3">
+        <v>313</v>
+      </c>
+      <c r="H16" s="3">
+        <v>19751</v>
+      </c>
+      <c r="I16" s="3">
+        <v>127</v>
+      </c>
+      <c r="J16" s="3">
         <v>84</v>
       </c>
-      <c r="K11" s="5">
-        <v>58</v>
-      </c>
-      <c r="L11" s="5">
-        <v>269</v>
-      </c>
-      <c r="M11" s="5">
-        <v>192</v>
-      </c>
-      <c r="N11" s="5">
-        <v>59</v>
-      </c>
-      <c r="O11" s="5">
-        <v>23</v>
-      </c>
-      <c r="P11" s="5">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="5">
-        <v>136615</v>
-      </c>
-      <c r="C12" s="5">
-        <v>4175</v>
-      </c>
-      <c r="D12" s="5">
-        <v>77984</v>
-      </c>
-      <c r="E12" s="5">
-        <v>838</v>
-      </c>
-      <c r="F12" s="5">
-        <v>125</v>
-      </c>
-      <c r="G12" s="5">
-        <v>5075</v>
-      </c>
-      <c r="H12" s="5">
-        <v>30956</v>
-      </c>
-      <c r="I12" s="5">
-        <v>16106</v>
-      </c>
-      <c r="J12" s="5">
-        <v>883</v>
-      </c>
-      <c r="K12" s="5">
-        <v>149</v>
-      </c>
-      <c r="L12" s="5">
-        <v>282</v>
-      </c>
-      <c r="M12" s="5">
-        <v>17</v>
-      </c>
-      <c r="N12" s="5">
-        <v>2</v>
-      </c>
-      <c r="O12" s="6" t="s">
+      <c r="K16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="5">
-        <v>56287</v>
-      </c>
-      <c r="C13" s="5">
-        <v>2031</v>
-      </c>
-      <c r="D13" s="5">
-        <v>38161</v>
-      </c>
-      <c r="E13" s="5">
-        <v>205</v>
-      </c>
-      <c r="F13" s="5">
-        <v>106</v>
-      </c>
-      <c r="G13" s="5">
-        <v>259</v>
-      </c>
-      <c r="H13" s="5">
-        <v>9667</v>
-      </c>
-      <c r="I13" s="5">
-        <v>1739</v>
-      </c>
-      <c r="J13" s="5">
-        <v>146</v>
-      </c>
-      <c r="K13" s="5">
-        <v>39</v>
-      </c>
-      <c r="L13" s="5">
-        <v>743</v>
-      </c>
-      <c r="M13" s="5">
-        <v>690</v>
-      </c>
-      <c r="N13" s="5">
-        <v>328</v>
-      </c>
-      <c r="O13" s="5">
-        <v>82</v>
-      </c>
-      <c r="P13" s="5">
-        <v>2091</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="L16" s="3">
+        <v>67</v>
+      </c>
+      <c r="M16" s="3">
+        <v>22</v>
+      </c>
+      <c r="N16" s="3">
+        <v>61</v>
+      </c>
+      <c r="O16" s="3">
+        <v>35</v>
+      </c>
+      <c r="P16" s="3">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5">
-        <v>83191</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1135</v>
-      </c>
-      <c r="D14" s="5">
-        <v>35156</v>
-      </c>
-      <c r="E14" s="5">
-        <v>723</v>
-      </c>
-      <c r="F14" s="5">
-        <v>222</v>
-      </c>
-      <c r="G14" s="5">
-        <v>1617</v>
-      </c>
-      <c r="H14" s="5">
-        <v>21082</v>
-      </c>
-      <c r="I14" s="5">
-        <v>16736</v>
-      </c>
-      <c r="J14" s="5">
-        <v>1063</v>
-      </c>
-      <c r="K14" s="5">
-        <v>192</v>
-      </c>
-      <c r="L14" s="5">
-        <v>489</v>
-      </c>
-      <c r="M14" s="5">
-        <v>61</v>
-      </c>
-      <c r="N14" s="5">
-        <v>96</v>
-      </c>
-      <c r="O14" s="5">
-        <v>24</v>
-      </c>
-      <c r="P14" s="5">
-        <v>4595</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="5">
-        <v>72218</v>
-      </c>
-      <c r="C15" s="5">
-        <v>6617</v>
-      </c>
-      <c r="D15" s="5">
-        <v>45178</v>
-      </c>
-      <c r="E15" s="5">
-        <v>613</v>
-      </c>
-      <c r="F15" s="5">
-        <v>120</v>
-      </c>
-      <c r="G15" s="5">
-        <v>162</v>
-      </c>
-      <c r="H15" s="5">
-        <v>14982</v>
-      </c>
-      <c r="I15" s="5">
-        <v>4041</v>
-      </c>
-      <c r="J15" s="5">
-        <v>143</v>
-      </c>
-      <c r="K15" s="5">
-        <v>2</v>
-      </c>
-      <c r="L15" s="5">
-        <v>129</v>
-      </c>
-      <c r="M15" s="5">
-        <v>89</v>
-      </c>
-      <c r="N15" s="5">
-        <v>7</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P15" s="5">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="5">
-        <v>54533</v>
-      </c>
-      <c r="C16" s="5">
-        <v>5598</v>
-      </c>
-      <c r="D16" s="5">
-        <v>26944</v>
-      </c>
-      <c r="E16" s="5">
-        <v>71</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="5">
-        <v>313</v>
-      </c>
-      <c r="H16" s="5">
-        <v>19751</v>
-      </c>
-      <c r="I16" s="5">
-        <v>127</v>
-      </c>
-      <c r="J16" s="5">
-        <v>84</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="5">
-        <v>67</v>
-      </c>
-      <c r="M16" s="5">
-        <v>22</v>
-      </c>
-      <c r="N16" s="5">
-        <v>61</v>
-      </c>
-      <c r="O16" s="5">
-        <v>35</v>
-      </c>
-      <c r="P16" s="5">
-        <v>1460</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="A20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
+      <c r="A24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
+      <c r="A28" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
+      <c r="A32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
@@ -1554,27 +1557,27 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>